<commit_message>
re-did the sockets, keep thing inside react
</commit_message>
<xml_diff>
--- a/DudoEvents.xlsx
+++ b/DudoEvents.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_NewDudo\Dudo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27A65A7-7F5C-42D4-AF12-A22C22086D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01ECEF9-166A-40CF-8DD9-C2C9034A349A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="26">
   <si>
     <t>server.js</t>
   </si>
@@ -88,6 +88,21 @@
   </si>
   <si>
     <t>joinLobby</t>
+  </si>
+  <si>
+    <t>connection</t>
+  </si>
+  <si>
+    <t>yourSocketId</t>
+  </si>
+  <si>
+    <t>callback 'lobby'</t>
+  </si>
+  <si>
+    <t>rejoinLobby</t>
+  </si>
+  <si>
+    <t>nextRound</t>
   </si>
 </sst>
 </file>
@@ -137,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -361,17 +376,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -415,42 +419,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,9 +732,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K11"/>
+  <dimension ref="B1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -751,26 +754,26 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="17" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="23"/>
+      <c r="F2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="17" t="s">
+      <c r="G2" s="23"/>
+      <c r="H2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="17" t="s">
+      <c r="I2" s="23"/>
+      <c r="J2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="18"/>
+      <c r="K2" s="23"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
@@ -805,35 +808,35 @@
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="29"/>
+      <c r="B4" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="27"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="G5" s="8" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="8"/>
@@ -842,91 +845,77 @@
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="8"/>
+      <c r="G6" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="H6" s="7"/>
-      <c r="I6" s="8" t="s">
-        <v>4</v>
-      </c>
+      <c r="I6" s="8"/>
       <c r="J6" s="1"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>10</v>
+      <c r="B7" s="5"/>
+      <c r="C7" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E7" s="8"/>
       <c r="F7" s="7"/>
       <c r="G7" s="8"/>
-      <c r="H7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="8"/>
       <c r="J7" s="1"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="30"/>
+      <c r="B8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="7"/>
       <c r="E9" s="8"/>
       <c r="F9" s="7"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="8"/>
       <c r="J9" s="1"/>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>7</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="7"/>
       <c r="G10" s="8"/>
       <c r="H10" s="7"/>
@@ -934,25 +923,149 @@
       <c r="J10" s="1"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="9" t="s">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="20"/>
+      <c r="C13" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="21"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C18" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E18" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="4"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -963,5 +1076,6 @@
     <mergeCell ref="J2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>